<commit_message>
Added Feature to Save files as .pdf and minor Formatting done using openpyxl
</commit_message>
<xml_diff>
--- a/EMAPP/Book1.xlsx
+++ b/EMAPP/Book1.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internship\Siemens\EMAPP\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{15267E9E-4E7D-4171-9262-836EF62CCD89}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7545" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Sheet1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3, National Hwy 9, Premnagar, </t>
+  </si>
+  <si>
+    <t>Ashok Nagar, Pune, Maharashtra 411016</t>
   </si>
   <si>
     <t>From:</t>
@@ -44,32 +44,44 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Total Consumption</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
+  </numFmts>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -81,7 +93,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -126,89 +138,310 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick"/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="36">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf borderId="6" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="9" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="10" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="13" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="14" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="15" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="16" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="17" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="18" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="10" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="19" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="11" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="14" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="16" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="20" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="20" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>19718</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A011D0DF-FA94-4DAF-B945-72F7CF23BF95}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1828800" cy="952500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="1" name="Image 1"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1848518" cy="1143000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -507,84 +740,224 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B4" sqref="B4:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="6" width="14"/>
+    <col customWidth="1" max="2" min="2" style="6" width="18.7109375"/>
+    <col customWidth="1" max="3" min="3" style="6" width="20.140625"/>
+    <col customWidth="1" max="4" min="4" style="6" width="17.28515625"/>
+    <col customWidth="1" max="5" min="5" style="6" width="16.5703125"/>
+    <col customWidth="1" max="6" min="6" style="6" width="15.28515625"/>
+    <col customWidth="1" max="7" min="7" style="6" width="18.28515625"/>
+    <col customWidth="1" max="8" min="8" style="6" width="14.85546875"/>
+    <col customWidth="1" max="9" min="9" style="6" width="16.140625"/>
+    <col customWidth="1" max="11" min="11" style="6" width="12.28515625"/>
+    <col customWidth="1" max="13" min="13" style="6" width="18.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="n"/>
+      <c r="B1" s="3" t="n"/>
+      <c r="C1" s="3" t="n"/>
+      <c r="D1" s="3" t="n"/>
+      <c r="E1" s="4" t="n"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="5" t="n"/>
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E6" s="2" t="s">
+      <c r="E2" s="29" t="n"/>
+      <c r="F2" s="1" t="n"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="5" t="n"/>
+      <c r="B3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="E3" s="29" t="n"/>
+      <c r="F3" s="1" t="n"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="5" t="n"/>
+      <c r="B4" s="21" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="3" t="s">
+      <c r="E4" s="29" t="n"/>
+      <c r="F4" s="1" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="5" s="6" spans="1:6" thickBot="1">
+      <c r="A5" s="5" t="n"/>
+      <c r="E5" s="7" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="6" s="6" spans="1:6" thickBot="1">
+      <c r="A6" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="B6" s="30" t="n">
+        <v>43101</v>
+      </c>
+      <c r="C6" s="27" t="n"/>
+      <c r="D6" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="E6" s="30" t="n">
+        <v>43251</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="7" s="6" spans="1:6" thickBot="1">
+      <c r="A7" s="5" t="n"/>
+      <c r="E7" s="7" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="8" s="6" spans="1:6" thickBot="1">
+      <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="C8" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="D8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="31" t="n">
+        <v>43101</v>
+      </c>
+      <c r="B9" s="13" t="n">
+        <v>940770.88</v>
+      </c>
+      <c r="C9" s="13" t="n">
+        <v>1771380.13</v>
+      </c>
+      <c r="D9" s="13" t="n">
+        <v>830609.2499999999</v>
+      </c>
+      <c r="E9" s="14" t="n">
+        <v>8306092.499999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="32" t="n">
+        <v>43132</v>
+      </c>
+      <c r="B10" s="11" t="n">
+        <v>1771380.13</v>
+      </c>
+      <c r="C10" s="11" t="n">
+        <v>2643781.5</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>872401.3700000001</v>
+      </c>
+      <c r="E10" s="16" t="n">
+        <v>8724013.700000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="32" t="n">
+        <v>43160</v>
+      </c>
+      <c r="B11" s="11" t="n">
+        <v>2643781.5</v>
+      </c>
+      <c r="C11" s="11" t="n">
+        <v>3736803</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <v>1093021.5</v>
+      </c>
+      <c r="E11" s="16" t="n">
+        <v>10930215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="32" t="n">
+        <v>43191</v>
+      </c>
+      <c r="B12" s="11" t="n">
+        <v>3736803</v>
+      </c>
+      <c r="C12" s="11" t="n">
+        <v>4921206</v>
+      </c>
+      <c r="D12" s="11" t="n">
+        <v>1184403</v>
+      </c>
+      <c r="E12" s="16" t="n">
+        <v>11844030</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="13" s="6" spans="1:6" thickBot="1">
+      <c r="A13" s="33" t="n">
+        <v>43221</v>
+      </c>
+      <c r="B13" s="18" t="n">
+        <v>4921206</v>
+      </c>
+      <c r="C13" s="18" t="n">
+        <v>6233259.5</v>
+      </c>
+      <c r="D13" s="18" t="n">
+        <v>1312053.5</v>
+      </c>
+      <c r="E13" s="19" t="n">
+        <v>13120535</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="14" s="6" spans="1:6" thickBot="1">
+      <c r="A14" s="5" t="n"/>
+      <c r="E14" s="7" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="15" s="6" spans="1:6" thickBot="1">
+      <c r="A15" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="35" t="n"/>
+      <c r="C15" s="35" t="n"/>
+      <c r="D15" s="35" t="n"/>
+      <c r="E15" s="20" t="n">
+        <v>5292488.62</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="16" s="6" spans="1:6" thickBot="1">
+      <c r="A16" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="35" t="n"/>
+      <c r="C16" s="35" t="n"/>
+      <c r="D16" s="35" t="n"/>
+      <c r="E16" s="26" t="n">
+        <v>52924886.2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="G4:K4"/>
+  <mergeCells count="5">
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>